<commit_message>
Plunger updated, spring added
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Component</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>many</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#9657k61/=x839tg</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E8"/>
+  <dimension ref="A4:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +510,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ready to test 3D print gear wheels
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Component</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>small iteration gear</t>
+  </si>
+  <si>
+    <t>Dowel alignment pins for gear</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#97155a426/=xwsf2k</t>
+  </si>
+  <si>
+    <t>1 pack</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E12"/>
+  <dimension ref="A4:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +602,20 @@
       </c>
       <c r="D12" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>